<commit_message>
update scrollable dan template excel
</commit_message>
<xml_diff>
--- a/public/templates/peserta.xlsx
+++ b/public/templates/peserta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fathurrohman/Proyek/honorarium/source-code/honorarium/public/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FATHUR\KERJAAN\Proyek-Honorarium\source-code\honorarium\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE133704-9F62-0E4E-9C71-E59B8EFD58B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2BE66B-2BF5-4858-8F6F-0CEE53AE4A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{674168BC-6BCF-C342-9E35-C2DEB8BAE251}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{674168BC-6BCF-C342-9E35-C2DEB8BAE251}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>ID</t>
   </si>
@@ -46,9 +46,6 @@
     <t>NIP</t>
   </si>
   <si>
-    <t>Pangkat/Golongan</t>
-  </si>
-  <si>
     <t>Jabatan</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
     <t>Bank</t>
   </si>
   <si>
-    <t>No Rekenin</t>
-  </si>
-  <si>
     <t>Ayam</t>
   </si>
   <si>
@@ -82,9 +76,6 @@
     <t>33333</t>
   </si>
   <si>
-    <t>III/a</t>
-  </si>
-  <si>
     <t>IV/d</t>
   </si>
   <si>
@@ -113,6 +104,66 @@
   </si>
   <si>
     <t>30303</t>
+  </si>
+  <si>
+    <t>No Rekening</t>
+  </si>
+  <si>
+    <t>Referensi Golongan/Ruang</t>
+  </si>
+  <si>
+    <t>Golongan/Ruang</t>
+  </si>
+  <si>
+    <t>I/A</t>
+  </si>
+  <si>
+    <t>I/B</t>
+  </si>
+  <si>
+    <t>I/C</t>
+  </si>
+  <si>
+    <t>I/D</t>
+  </si>
+  <si>
+    <t>II/A</t>
+  </si>
+  <si>
+    <t>II/B</t>
+  </si>
+  <si>
+    <t>II/C</t>
+  </si>
+  <si>
+    <t>II/D</t>
+  </si>
+  <si>
+    <t>III/A</t>
+  </si>
+  <si>
+    <t>III/B</t>
+  </si>
+  <si>
+    <t>III/C</t>
+  </si>
+  <si>
+    <t>III/D</t>
+  </si>
+  <si>
+    <t>IV/A</t>
+  </si>
+  <si>
+    <t>IV/B</t>
+  </si>
+  <si>
+    <t>IV/C</t>
+  </si>
+  <si>
+    <t>IV/D</t>
+  </si>
+  <si>
+    <t>IV/E</t>
   </si>
 </sst>
 </file>
@@ -176,11 +227,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -199,9 +251,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -239,7 +291,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -345,7 +397,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -487,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -495,19 +547,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236FD699-9766-F24C-9067-529CD1A244A0}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,108 +571,195 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="I3" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>25</v>
+      <c r="L4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L6" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L7" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L9" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L10" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L12" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L13" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L14" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L15" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L16" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L17" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L18" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Golongan/Ruang" error="Tidak Sesuai, Lihat kolom Referensi" sqref="D1:D1048576" xr:uid="{A871D71D-90A9-4A1E-8D34-27623209F0FB}">
+      <formula1>$L$2:$L$18</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
enhance parse-excel-on-server, treat allowedColumns
</commit_message>
<xml_diff>
--- a/public/templates/peserta.xlsx
+++ b/public/templates/peserta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FATHUR\KERJAAN\Proyek-Honorarium\source-code\honorarium\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fathurrohman/Proyek/honorarium/source-code/honorarium/public/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2BE66B-2BF5-4858-8F6F-0CEE53AE4A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60193F3A-D56C-194F-981D-76B4EA4594F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{674168BC-6BCF-C342-9E35-C2DEB8BAE251}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19500" xr2:uid="{674168BC-6BCF-C342-9E35-C2DEB8BAE251}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,8 +34,27 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={EFDE4582-78C8-DA47-82C6-ADBB549459CF}</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{EFDE4582-78C8-DA47-82C6-ADBB549459CF}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    I/A, I/B, I/C, I/D, II/A, II/B, II/C, II/D, III/A, III/B, III/C, III/D, IV/A, IV/B, IV/C, IV/D, IV/E
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -76,9 +95,6 @@
     <t>33333</t>
   </si>
   <si>
-    <t>IV/d</t>
-  </si>
-  <si>
     <t>III/c</t>
   </si>
   <si>
@@ -106,15 +122,12 @@
     <t>30303</t>
   </si>
   <si>
-    <t>No Rekening</t>
+    <t>Golongan/Ruang</t>
   </si>
   <si>
     <t>Referensi Golongan/Ruang</t>
   </si>
   <si>
-    <t>Golongan/Ruang</t>
-  </si>
-  <si>
     <t>I/A</t>
   </si>
   <si>
@@ -164,6 +177,15 @@
   </si>
   <si>
     <t>IV/E</t>
+  </si>
+  <si>
+    <t>Nomor Rekening</t>
+  </si>
+  <si>
+    <t>NIK</t>
+  </si>
+  <si>
+    <t>NPWP</t>
   </si>
 </sst>
 </file>
@@ -227,12 +249,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -250,10 +271,16 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Fathur Rohman" id="{0C2D1CD6-5D30-304C-8686-F7A0B5EA83C9}" userId="fcdc85e8c3fcf2cd" providerId="Windows Live"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -291,7 +318,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -397,7 +424,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -539,28 +566,42 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="F1" dT="2024-08-27T22:21:08.38" personId="{0C2D1CD6-5D30-304C-8686-F7A0B5EA83C9}" id="{EFDE4582-78C8-DA47-82C6-ADBB549459CF}">
+    <text xml:space="preserve">I/A, I/B, I/C, I/D, II/A, II/B, II/C, II/D, III/A, III/B, III/C, III/D, IV/A, IV/B, IV/C, IV/D, IV/E
+</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236FD699-9766-F24C-9067-529CD1A244A0}">
-  <dimension ref="A1:L18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236FD699-9766-F24C-9067-529CD1A244A0}">
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,28 +612,34 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -602,27 +649,33 @@
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="2"/>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -632,29 +685,35 @@
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -664,102 +723,109 @@
       <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="2" t="s">
+      <c r="K4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L5" s="2" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L6" s="2" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L7" s="2" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L8" s="2" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L9" s="2" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L10" s="2" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L11" s="2" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L12" s="2" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L13" s="2" t="s">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L14" s="2" t="s">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L15" s="2" t="s">
+    <row r="17" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L16" s="2" t="s">
+    <row r="18" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O18" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L17" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L18" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Golongan/Ruang" error="Tidak Sesuai, Lihat kolom Referensi" sqref="D1:D1048576" xr:uid="{A871D71D-90A9-4A1E-8D34-27623209F0FB}">
-      <formula1>$L$2:$L$18</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Golongan/Ruang" error="Data tidak benar" sqref="F1:F1048576" xr:uid="{CBF6BBEA-9FEE-8D40-A62B-DF44C4B864C2}">
+      <formula1>$O$2:$O$18</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>